<commit_message>
Slight modifications to ISS
</commit_message>
<xml_diff>
--- a/model_data.xlsx
+++ b/model_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26985" windowHeight="18540" tabRatio="994" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26985" windowHeight="18540" tabRatio="994" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="SYS1" sheetId="1" r:id="rId1"/>
@@ -8423,7 +8423,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D198"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -8437,10 +8437,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -12130,7 +12130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
All models have been updated with the new tests
</commit_message>
<xml_diff>
--- a/model_data.xlsx
+++ b/model_data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shekar\Desktop\SFRAT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zakar\Desktop\Research\SFRAT\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F86EC8B-C7E4-4B30-A667-0D8E7876488B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26985" windowHeight="18540" tabRatio="994" activeTab="17"/>
+    <workbookView xWindow="5085" yWindow="3270" windowWidth="21600" windowHeight="11385" tabRatio="994" firstSheet="24" activeTab="39" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SYS1" sheetId="1" r:id="rId1"/>
@@ -43,19 +44,32 @@
     <sheet name="DATA10" sheetId="29" r:id="rId29"/>
     <sheet name="DATA11" sheetId="30" r:id="rId30"/>
     <sheet name="DATA12" sheetId="31" r:id="rId31"/>
-    <sheet name="DATA13" sheetId="32" r:id="rId32"/>
-    <sheet name="DATA14" sheetId="33" r:id="rId33"/>
-    <sheet name="JM_BM_Results" sheetId="34" r:id="rId34"/>
-    <sheet name="GM_BM_Results" sheetId="35" r:id="rId35"/>
-    <sheet name="GO_BM_FT" sheetId="36" r:id="rId36"/>
+    <sheet name="GO_BM_FT" sheetId="36" r:id="rId32"/>
+    <sheet name="DATA13" sheetId="32" r:id="rId33"/>
+    <sheet name="DATA14" sheetId="33" r:id="rId34"/>
+    <sheet name="JM_BM_Results" sheetId="34" r:id="rId35"/>
+    <sheet name="GM_BM_Results" sheetId="35" r:id="rId36"/>
     <sheet name="GO_EM_FT" sheetId="37" r:id="rId37"/>
+    <sheet name="DSS" sheetId="38" r:id="rId38"/>
+    <sheet name="ISS" sheetId="40" r:id="rId39"/>
+    <sheet name="Weibull" sheetId="39" r:id="rId40"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="68">
   <si>
     <t>FN</t>
   </si>
@@ -207,9 +221,6 @@
     <t>DATA14</t>
   </si>
   <si>
-    <t>Data.set</t>
-  </si>
-  <si>
     <t>D0</t>
   </si>
   <si>
@@ -233,15 +244,45 @@
   <si>
     <t>a</t>
   </si>
+  <si>
+    <t>DSS (aMLEs)</t>
+  </si>
+  <si>
+    <t>DSS (bMLEs)</t>
+  </si>
+  <si>
+    <t>S2IF</t>
+  </si>
+  <si>
+    <t>S2FC</t>
+  </si>
+  <si>
+    <t>a (MLE)</t>
+  </si>
+  <si>
+    <t>b (MLE)</t>
+  </si>
+  <si>
+    <t>c (MLE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diverging </t>
+  </si>
+  <si>
+    <t>2.13331*10^7</t>
+  </si>
+  <si>
+    <t>2.84101*10^7</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -272,6 +313,11 @@
       <name val="Arial"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -301,7 +347,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -321,6 +367,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -673,11 +720,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C137"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -2336,7 +2383,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2857,7 +2904,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:C115"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4254,7 +4301,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:C74"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5159,7 +5206,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5838,10 +5885,12 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <sheetData>
@@ -6515,7 +6564,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6808,7 +6857,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7498,7 +7547,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:C82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8420,14 +8469,17 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:D198"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="3" max="3" width="20" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -11606,7 +11658,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -12127,7 +12179,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13190,7 +13242,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13473,7 +13525,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13840,7 +13892,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14111,7 +14163,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14449,7 +14501,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14600,7 +14652,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14787,7 +14839,7 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:C110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16126,7 +16178,7 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:C112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17488,7 +17540,7 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:C200"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19907,7 +19959,7 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20130,11 +20182,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C208"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -22645,7 +22697,7 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:C119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -24092,7 +24144,7 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:B181"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -25560,7 +25612,438 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
+  <dimension ref="A1:H32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1">
+        <v>3.4203784064249599E-5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>142.880914316195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1.5671038156473599E-5</v>
+      </c>
+      <c r="C3" s="1">
+        <v>107.545299197475</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1">
+        <v>9.8650123103193301E-5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>256.62528828760497</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2.5759629688921801E-2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>527.29465836991301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2.1406133731007501E-5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>402.04658084005302</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.0551705931084401E-5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>478.80082295570401</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1">
+        <v>4.14377154545155E-5</v>
+      </c>
+      <c r="C8" s="1">
+        <v>43.197636126106303</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2.67171059071668E-5</v>
+      </c>
+      <c r="C9" s="1">
+        <v>57.129778868783603</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1">
+        <v>5.9019615150453196E-3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>435.467707382171</v>
+      </c>
+      <c r="F10">
+        <v>-3.3218953455390499E-2</v>
+      </c>
+      <c r="G10">
+        <v>-651.06479851736901</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="2">
+        <v>5.74179296554284E-3</v>
+      </c>
+      <c r="C11" s="2">
+        <v>347.14240588184998</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3">
+        <v>-1.2997000250156199E-2</v>
+      </c>
+      <c r="G11" s="3">
+        <v>-2509.73442796876</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="1">
+        <v>4.5172529474652397E-2</v>
+      </c>
+      <c r="C12" s="1">
+        <v>418.103928617002</v>
+      </c>
+      <c r="F12">
+        <v>-4.1311071839082003E-2</v>
+      </c>
+      <c r="G12">
+        <v>-2142.8587322319099</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="2">
+        <v>-1.08125995637951E-2</v>
+      </c>
+      <c r="C13" s="2">
+        <v>-77.653829737787305</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3">
+        <v>-2.70677312776893E-2</v>
+      </c>
+      <c r="G13" s="3">
+        <v>-416.36245605928502</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="1">
+        <v>3.5136503233212002E-3</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1625.41115427865</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="1">
+        <v>6.2489229435537595E-4</v>
+      </c>
+      <c r="C15" s="1">
+        <v>69.537757021361301</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="1">
+        <v>3.5416020529530103E-5</v>
+      </c>
+      <c r="C16" s="1">
+        <v>142.86928835535301</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="2">
+        <v>-2.6511414347945E-2</v>
+      </c>
+      <c r="C17" s="2">
+        <v>-63.712277856458599</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3">
+        <v>-0.121526317320517</v>
+      </c>
+      <c r="G17" s="3">
+        <v>-39.549007926474999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2.5386904323510099E-2</v>
+      </c>
+      <c r="C18" s="1">
+        <v>469.97371142259999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="2">
+        <v>469.97371142259999</v>
+      </c>
+      <c r="C19" s="2">
+        <v>326.410902310133</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3">
+        <v>-7.44589172856433E-2</v>
+      </c>
+      <c r="G19" s="3">
+        <v>-1047.4192190824101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="1">
+        <v>8.0001587169268501E-2</v>
+      </c>
+      <c r="C20" s="1">
+        <v>4963.6567591317098</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1.9950080586073799E-2</v>
+      </c>
+      <c r="C21" s="1">
+        <v>605.56551537942403</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="1">
+        <v>3.0692045732278399E-2</v>
+      </c>
+      <c r="C22" s="1">
+        <v>497.753963416494</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="2">
+        <v>-3.6275134780990501E-3</v>
+      </c>
+      <c r="C23" s="2">
+        <v>-58.591238007076598</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3">
+        <v>-1.38402737860679E-2</v>
+      </c>
+      <c r="G23" s="3">
+        <v>-367.40169043975101</v>
+      </c>
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="1">
+        <v>7.8812691755874003E-3</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1696.14966306473</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1.5846835246707699E-2</v>
+      </c>
+      <c r="C25" s="1">
+        <v>162.69642762348701</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="1">
+        <v>4.4514493816366898E-3</v>
+      </c>
+      <c r="C26" s="1">
+        <v>350.37897700834202</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="1">
+        <v>4.3307462405919803E-3</v>
+      </c>
+      <c r="C27" s="1">
+        <v>350.57916352834599</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="1">
+        <v>2.6921515652162602E-2</v>
+      </c>
+      <c r="C28" s="1">
+        <v>383.98265342307099</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="1">
+        <v>4.2185937148540597E-5</v>
+      </c>
+      <c r="C29" s="1">
+        <v>401.057135585521</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="1">
+        <v>3.8992934365107498E-5</v>
+      </c>
+      <c r="C30" s="1">
+        <v>133.13476719799399</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1.3774059979412999E-4</v>
+      </c>
+      <c r="C31" s="1">
+        <v>118.23445463328</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1">
+        <v>4.5172529474652397E-2</v>
+      </c>
+      <c r="C32" s="1">
+        <v>418.103928617002</v>
+      </c>
+      <c r="F32">
+        <v>-4.1311071839082003E-2</v>
+      </c>
+      <c r="G32">
+        <v>-2142.8587322319099</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:B214"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -27289,8 +27772,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -27872,15 +28355,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="4" t="s">
@@ -28240,13 +28726,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
@@ -28254,11 +28738,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
         <v>50</v>
-      </c>
-      <c r="B1" t="s">
-        <v>51</v>
       </c>
       <c r="C1" t="s">
         <v>12</v>
@@ -28611,462 +29095,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T80" sqref="T80"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="1">
-        <v>3.4203784064249599E-5</v>
-      </c>
-      <c r="C2" s="1">
-        <v>142.880914316195</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1.5671038156473599E-5</v>
-      </c>
-      <c r="C3" s="1">
-        <v>107.545299197475</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="1">
-        <v>9.8650123103193301E-5</v>
-      </c>
-      <c r="C4" s="1">
-        <v>256.62528828760497</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="1">
-        <v>2.5759629688921801E-2</v>
-      </c>
-      <c r="C5" s="1">
-        <v>527.29465836991301</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2.1406133731007501E-5</v>
-      </c>
-      <c r="C6" s="1">
-        <v>402.04658084005302</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1.0551705931084401E-5</v>
-      </c>
-      <c r="C7" s="1">
-        <v>478.80082295570401</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="1">
-        <v>4.14377154545155E-5</v>
-      </c>
-      <c r="C8" s="1">
-        <v>43.197636126106303</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2.67171059071668E-5</v>
-      </c>
-      <c r="C9" s="1">
-        <v>57.129778868783603</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="1">
-        <v>5.9019615150453196E-3</v>
-      </c>
-      <c r="C10" s="1">
-        <v>435.467707382171</v>
-      </c>
-      <c r="F10">
-        <v>-3.3218953455390499E-2</v>
-      </c>
-      <c r="G10">
-        <v>-651.06479851736901</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="2">
-        <v>5.74179296554284E-3</v>
-      </c>
-      <c r="C11" s="2">
-        <v>347.14240588184998</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3">
-        <v>-1.2997000250156199E-2</v>
-      </c>
-      <c r="G11" s="3">
-        <v>-2509.73442796876</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="1">
-        <v>4.5172529474652397E-2</v>
-      </c>
-      <c r="C12" s="1">
-        <v>418.103928617002</v>
-      </c>
-      <c r="F12">
-        <v>-4.1311071839082003E-2</v>
-      </c>
-      <c r="G12">
-        <v>-2142.8587322319099</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="2">
-        <v>-1.08125995637951E-2</v>
-      </c>
-      <c r="C13" s="2">
-        <v>-77.653829737787305</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3">
-        <v>-2.70677312776893E-2</v>
-      </c>
-      <c r="G13" s="3">
-        <v>-416.36245605928502</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="1">
-        <v>3.5136503233212002E-3</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1625.41115427865</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="1">
-        <v>6.2489229435537595E-4</v>
-      </c>
-      <c r="C15" s="1">
-        <v>69.537757021361301</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="1">
-        <v>3.5416020529530103E-5</v>
-      </c>
-      <c r="C16" s="1">
-        <v>142.86928835535301</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="2">
-        <v>-2.6511414347945E-2</v>
-      </c>
-      <c r="C17" s="2">
-        <v>-63.712277856458599</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3">
-        <v>-0.121526317320517</v>
-      </c>
-      <c r="G17" s="3">
-        <v>-39.549007926474999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="1">
-        <v>2.5386904323510099E-2</v>
-      </c>
-      <c r="C18" s="1">
-        <v>469.97371142259999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="2">
-        <v>469.97371142259999</v>
-      </c>
-      <c r="C19" s="2">
-        <v>326.410902310133</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3">
-        <v>-7.44589172856433E-2</v>
-      </c>
-      <c r="G19" s="3">
-        <v>-1047.4192190824101</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="1">
-        <v>8.0001587169268501E-2</v>
-      </c>
-      <c r="C20" s="1">
-        <v>4963.6567591317098</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="1">
-        <v>1.9950080586073799E-2</v>
-      </c>
-      <c r="C21" s="1">
-        <v>605.56551537942403</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="1">
-        <v>3.0692045732278399E-2</v>
-      </c>
-      <c r="C22" s="1">
-        <v>497.753963416494</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="2">
-        <v>-3.6275134780990501E-3</v>
-      </c>
-      <c r="C23" s="2">
-        <v>-58.591238007076598</v>
-      </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3">
-        <v>-1.38402737860679E-2</v>
-      </c>
-      <c r="G23" s="3">
-        <v>-367.40169043975101</v>
-      </c>
-      <c r="H23" s="3"/>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="1">
-        <v>7.8812691755874003E-3</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1696.14966306473</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="1">
-        <v>1.5846835246707699E-2</v>
-      </c>
-      <c r="C25" s="1">
-        <v>162.69642762348701</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="1">
-        <v>4.4514493816366898E-3</v>
-      </c>
-      <c r="C26" s="1">
-        <v>350.37897700834202</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="1">
-        <v>4.3307462405919803E-3</v>
-      </c>
-      <c r="C27" s="1">
-        <v>350.57916352834599</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="1">
-        <v>2.6921515652162602E-2</v>
-      </c>
-      <c r="C28" s="1">
-        <v>383.98265342307099</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" s="1">
-        <v>4.2185937148540597E-5</v>
-      </c>
-      <c r="C29" s="1">
-        <v>401.057135585521</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B30" s="1">
-        <v>3.8992934365107498E-5</v>
-      </c>
-      <c r="C30" s="1">
-        <v>133.13476719799399</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B31" s="1">
-        <v>1.3774059979412999E-4</v>
-      </c>
-      <c r="C31" s="1">
-        <v>118.23445463328</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B32" s="1">
-        <v>4.5172529474652397E-2</v>
-      </c>
-      <c r="C32" s="1">
-        <v>418.103928617002</v>
-      </c>
-      <c r="F32">
-        <v>-4.1311071839082003E-2</v>
-      </c>
-      <c r="G32">
-        <v>-2142.8587322319099</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -29416,8 +29465,893 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCF81ECE-5A5C-41EB-9308-A467968527CE}">
+  <dimension ref="A1:C35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15">
+      <c r="A1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15">
+      <c r="A2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="11">
+        <v>136.994</v>
+      </c>
+      <c r="C2" s="11">
+        <v>7.8998000000000005E-5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15">
+      <c r="A3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="11">
+        <v>90.0505</v>
+      </c>
+      <c r="C3" s="11">
+        <v>4.7485099999999997E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15">
+      <c r="A4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="11">
+        <v>216.33199999999999</v>
+      </c>
+      <c r="C4" s="11">
+        <v>2.9551399999999998E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15">
+      <c r="A5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="11">
+        <v>397.28300000000002</v>
+      </c>
+      <c r="C5" s="11">
+        <v>8.8253399999999998E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15">
+      <c r="A6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="11">
+        <v>129.506</v>
+      </c>
+      <c r="C6" s="11">
+        <v>8.6576200000000006E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15">
+      <c r="A7" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="11">
+        <v>106.581</v>
+      </c>
+      <c r="C7" s="11">
+        <v>3.6495499999999998E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15">
+      <c r="A8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="11">
+        <v>300.20400000000001</v>
+      </c>
+      <c r="C8" s="11">
+        <v>7.7645999999999995E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15">
+      <c r="A9" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="11">
+        <v>160.6</v>
+      </c>
+      <c r="C9" s="11">
+        <v>5.1531899999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15">
+      <c r="A10" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="11">
+        <v>244.81100000000001</v>
+      </c>
+      <c r="C10" s="11">
+        <v>2.2612400000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15">
+      <c r="A11" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="11">
+        <v>362.62099999999998</v>
+      </c>
+      <c r="C11" s="11">
+        <v>0.128721</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15">
+      <c r="A12" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="11">
+        <v>591.25900000000001</v>
+      </c>
+      <c r="C12" s="11">
+        <v>1.0057200000000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15">
+      <c r="A13" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="11">
+        <v>454.89400000000001</v>
+      </c>
+      <c r="C13" s="11">
+        <v>4.1647099999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15">
+      <c r="A14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="11">
+        <v>54.471800000000002</v>
+      </c>
+      <c r="C14" s="11">
+        <v>6.2584700000000004E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15">
+      <c r="A15" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="11">
+        <v>54.485399999999998</v>
+      </c>
+      <c r="C15" s="11">
+        <v>0.30777500000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15">
+      <c r="A16" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="11">
+        <v>54.485399999999998</v>
+      </c>
+      <c r="C16" s="11">
+        <v>0.30777500000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15">
+      <c r="A17" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="11">
+        <v>41.323500000000003</v>
+      </c>
+      <c r="C17" s="11">
+        <v>9.6267600000000006E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15">
+      <c r="A18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="11">
+        <v>472.637</v>
+      </c>
+      <c r="C18" s="11">
+        <v>6.9007799999999994E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15">
+      <c r="A19" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="11">
+        <v>300.20400000000001</v>
+      </c>
+      <c r="C19" s="11">
+        <v>7.7645999999999995E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15">
+      <c r="A20" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="11">
+        <v>231.30699999999999</v>
+      </c>
+      <c r="C20" s="11">
+        <v>6.7421800000000006E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15">
+      <c r="A21" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="11">
+        <v>362.62099999999998</v>
+      </c>
+      <c r="C21" s="11">
+        <v>0.128721</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15">
+      <c r="A22" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="11">
+        <v>31.620999999999999</v>
+      </c>
+      <c r="C22" s="11">
+        <v>4.2899599999999998E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15">
+      <c r="A23" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="11">
+        <v>136.75899999999999</v>
+      </c>
+      <c r="C23" s="11">
+        <v>8.2450399999999999E-5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15">
+      <c r="A24" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="11">
+        <v>71.767700000000005</v>
+      </c>
+      <c r="C24" s="11">
+        <v>0.103893</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15">
+      <c r="A25" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="11">
+        <v>351.94</v>
+      </c>
+      <c r="C25" s="11">
+        <v>9.1677400000000006E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15">
+      <c r="A26" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="11">
+        <v>287.16000000000003</v>
+      </c>
+      <c r="C26" s="11">
+        <v>0.41694300000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15">
+      <c r="A27" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="11">
+        <v>3510.9</v>
+      </c>
+      <c r="C27" s="11">
+        <v>0.31310300000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15">
+      <c r="A28" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="11">
+        <v>546.83000000000004</v>
+      </c>
+      <c r="C28" s="11">
+        <v>5.2677000000000002E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15">
+      <c r="A29" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="11">
+        <v>483.05099999999999</v>
+      </c>
+      <c r="C29" s="11">
+        <v>6.8604299999999993E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15">
+      <c r="A30" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="11">
+        <v>76.066500000000005</v>
+      </c>
+      <c r="C30" s="11">
+        <v>1.28202E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15">
+      <c r="A31" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="11">
+        <v>248.798</v>
+      </c>
+      <c r="C31" s="11">
+        <v>0.18542</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15">
+      <c r="A32" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="11">
+        <v>125.68300000000001</v>
+      </c>
+      <c r="C32" s="11">
+        <v>5.4630499999999999E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15">
+      <c r="A33" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="1:3" ht="15">
+      <c r="A34" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="1:3" ht="15">
+      <c r="A35" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" s="11">
+        <v>281.64299999999997</v>
+      </c>
+      <c r="C35" s="11">
+        <v>0.100354</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5895E50-6561-49A6-B8DA-395B361E4A9A}">
+  <dimension ref="A1:E35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>136</v>
+      </c>
+      <c r="C2">
+        <v>4.0404600000000003E-5</v>
+      </c>
+      <c r="D2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>86</v>
+      </c>
+      <c r="C3">
+        <v>2.62402E-5</v>
+      </c>
+      <c r="D3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>207</v>
+      </c>
+      <c r="C4">
+        <v>1.6276600000000001E-4</v>
+      </c>
+      <c r="D4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>397</v>
+      </c>
+      <c r="C5">
+        <v>4.4263900000000002E-5</v>
+      </c>
+      <c r="D5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>129</v>
+      </c>
+      <c r="C6">
+        <v>4.3875599999999997E-5</v>
+      </c>
+      <c r="D6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>104</v>
+      </c>
+      <c r="C7">
+        <v>1.9393399999999999E-4</v>
+      </c>
+      <c r="D7">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>278</v>
+      </c>
+      <c r="C8">
+        <v>4.5037499999999997E-5</v>
+      </c>
+      <c r="D8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9">
+        <v>176.852</v>
+      </c>
+      <c r="C9">
+        <v>3.8736600000000003E-2</v>
+      </c>
+      <c r="D9">
+        <v>2.3109000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10">
+        <v>213.72399999999999</v>
+      </c>
+      <c r="C10">
+        <v>4.4701600000000001E-2</v>
+      </c>
+      <c r="D10">
+        <v>23.9621</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11">
+        <v>616.48199999999997</v>
+      </c>
+      <c r="C11">
+        <v>1.6882799999999999E-4</v>
+      </c>
+      <c r="D11">
+        <v>-0.99454100000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12">
+        <v>242.39500000000001</v>
+      </c>
+      <c r="C12">
+        <v>3.8062199999999997E-2</v>
+      </c>
+      <c r="D12">
+        <v>20.884899999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13">
+        <v>577.50599999999997</v>
+      </c>
+      <c r="C13">
+        <v>2.3827299999999999E-2</v>
+      </c>
+      <c r="D13">
+        <v>1.69235</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14">
+        <v>54</v>
+      </c>
+      <c r="C14">
+        <v>3.2124800000000001E-5</v>
+      </c>
+      <c r="D14">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15">
+        <v>54</v>
+      </c>
+      <c r="C15">
+        <v>3.2124800000000001E-5</v>
+      </c>
+      <c r="D15">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16">
+        <v>54</v>
+      </c>
+      <c r="C16">
+        <v>1.58382</v>
+      </c>
+      <c r="D16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17">
+        <v>41</v>
+      </c>
+      <c r="C17">
+        <v>4.93098E-5</v>
+      </c>
+      <c r="D17">
+        <v>0.1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>493.44900000000001</v>
+      </c>
+      <c r="C18">
+        <v>3.9980700000000001E-2</v>
+      </c>
+      <c r="D18">
+        <v>0.72408399999999995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>278</v>
+      </c>
+      <c r="C19">
+        <v>4.5037499999999997E-5</v>
+      </c>
+      <c r="D19">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>197</v>
+      </c>
+      <c r="C20">
+        <v>4.3649799999999997E-5</v>
+      </c>
+      <c r="D20">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21">
+        <v>616.48199999999997</v>
+      </c>
+      <c r="C21">
+        <v>1.6882799999999999E-4</v>
+      </c>
+      <c r="D21">
+        <v>-0.99454100000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22">
+        <v>37.456699999999998</v>
+      </c>
+      <c r="C22">
+        <v>1.7443999999999999E-3</v>
+      </c>
+      <c r="D22">
+        <v>0.445685</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23">
+        <v>135.99799999999999</v>
+      </c>
+      <c r="C23">
+        <v>2.4680900000000001E-4</v>
+      </c>
+      <c r="D23">
+        <v>31513.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24">
+        <v>56.576500000000003</v>
+      </c>
+      <c r="C24">
+        <v>0.178562</v>
+      </c>
+      <c r="D24">
+        <v>6.9463200000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25">
+        <v>352.83600000000001</v>
+      </c>
+      <c r="C25">
+        <v>8.2778299999999999E-2</v>
+      </c>
+      <c r="D25">
+        <v>2.8348399999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26">
+        <v>279</v>
+      </c>
+      <c r="C26">
+        <v>2.6728000000000001</v>
+      </c>
+      <c r="D26" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27">
+        <v>3675.03</v>
+      </c>
+      <c r="C27">
+        <v>0.232907</v>
+      </c>
+      <c r="D27">
+        <v>1.8679600000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28">
+        <v>540.23199999999997</v>
+      </c>
+      <c r="C28">
+        <v>5.9503800000000003E-2</v>
+      </c>
+      <c r="D28">
+        <v>5.4038899999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29">
+        <v>482.01600000000002</v>
+      </c>
+      <c r="C29">
+        <v>7.03038E-2</v>
+      </c>
+      <c r="D29">
+        <v>4.1743600000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30">
+        <v>58.0276</v>
+      </c>
+      <c r="C30">
+        <v>3.0598500000000001E-2</v>
+      </c>
+      <c r="D30">
+        <v>23.222000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31">
+        <v>208.62899999999999</v>
+      </c>
+      <c r="C31">
+        <v>0.35881800000000003</v>
+      </c>
+      <c r="D31">
+        <v>15.6629</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>46</v>
+      </c>
+      <c r="E32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>47</v>
+      </c>
+      <c r="E33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35">
+        <v>302.87400000000002</v>
+      </c>
+      <c r="C35">
+        <v>5.9592399999999997E-2</v>
+      </c>
+      <c r="D35">
+        <v>1.0109399999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C398"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -34211,8 +35145,500 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05E0387C-22BF-42E8-B1BA-F2B3AB1E56DA}">
+  <dimension ref="A1:E35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="2" max="2" width="42.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>172.52600000000001</v>
+      </c>
+      <c r="C2">
+        <v>6.9605700000000003E-4</v>
+      </c>
+      <c r="D2">
+        <v>0.67673899999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>139.953</v>
+      </c>
+      <c r="C3">
+        <v>7.2103799999999999E-5</v>
+      </c>
+      <c r="D3">
+        <v>0.82241600000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>281.51100000000002</v>
+      </c>
+      <c r="C4">
+        <v>1.8371500000000001E-4</v>
+      </c>
+      <c r="D4">
+        <v>0.91422199999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>-32.572499999999998</v>
+      </c>
+      <c r="C5">
+        <v>-0.366035</v>
+      </c>
+      <c r="D5">
+        <v>0.168351</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>137.63</v>
+      </c>
+      <c r="C6">
+        <v>1.71457E-4</v>
+      </c>
+      <c r="D6">
+        <v>0.85021500000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <f>-6.69106*10^16</f>
+        <v>-6.69106E+16</v>
+      </c>
+      <c r="C7">
+        <f>-3.67959*10^10</f>
+        <v>-36795900000</v>
+      </c>
+      <c r="D7">
+        <v>-6.06487</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>518.29600000000005</v>
+      </c>
+      <c r="C8">
+        <v>4.88617E-5</v>
+      </c>
+      <c r="D8">
+        <v>0.88542600000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9">
+        <v>374.29899999999998</v>
+      </c>
+      <c r="C9">
+        <v>7.08093E-3</v>
+      </c>
+      <c r="D9">
+        <v>0.999274</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10">
+        <v>4140.51</v>
+      </c>
+      <c r="C10">
+        <v>3.0728199999999998E-4</v>
+      </c>
+      <c r="D10">
+        <v>1.0009300000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11">
+        <v>529.73099999999999</v>
+      </c>
+      <c r="C11">
+        <v>2.6499700000000001E-2</v>
+      </c>
+      <c r="D11">
+        <v>1.0979399999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12">
+        <v>1170.8800000000001</v>
+      </c>
+      <c r="C12">
+        <v>1.5353000000000001E-3</v>
+      </c>
+      <c r="D12">
+        <v>0.99515200000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13">
+        <v>-28478.799999999999</v>
+      </c>
+      <c r="C13">
+        <v>-1.7540399999999999E-4</v>
+      </c>
+      <c r="D13">
+        <v>0.99993100000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14">
+        <v>67.207099999999997</v>
+      </c>
+      <c r="C14">
+        <v>4.46465E-4</v>
+      </c>
+      <c r="D14">
+        <v>0.70719299999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15">
+        <v>67.207099999999997</v>
+      </c>
+      <c r="C15">
+        <v>4.46465E-4</v>
+      </c>
+      <c r="D15">
+        <v>0.70719299999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16">
+        <v>54.558799999999998</v>
+      </c>
+      <c r="C16">
+        <v>0.208235</v>
+      </c>
+      <c r="D16">
+        <v>0.74129299999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17">
+        <v>45.578000000000003</v>
+      </c>
+      <c r="C17">
+        <v>1.8128400000000001E-4</v>
+      </c>
+      <c r="D17">
+        <v>0.84483600000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>571.05799999999999</v>
+      </c>
+      <c r="C18">
+        <v>2.0326899999999998E-2</v>
+      </c>
+      <c r="D18">
+        <v>1.06165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>518.29600000000005</v>
+      </c>
+      <c r="C19">
+        <v>4.88617E-5</v>
+      </c>
+      <c r="D19">
+        <v>0.88542600000000005</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>199.369</v>
+      </c>
+      <c r="C20">
+        <v>3.3154400000000002</v>
+      </c>
+      <c r="D20">
+        <v>2.6833699999999999E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21">
+        <v>529.73099999999999</v>
+      </c>
+      <c r="C21">
+        <v>2.6499700000000001E-2</v>
+      </c>
+      <c r="D21">
+        <v>1.0979399999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22">
+        <v>-51.443399999999997</v>
+      </c>
+      <c r="C22">
+        <v>-2.0090199999999999E-2</v>
+      </c>
+      <c r="D22">
+        <v>0.99924000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23">
+        <v>1268.73</v>
+      </c>
+      <c r="C23">
+        <v>4.0494800000000003E-3</v>
+      </c>
+      <c r="D23">
+        <v>1.0001800000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24">
+        <v>-94.670400000000001</v>
+      </c>
+      <c r="C24">
+        <v>-1.98009E-2</v>
+      </c>
+      <c r="D24">
+        <v>0.99855799999999995</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25">
+        <v>686.34699999999998</v>
+      </c>
+      <c r="C25">
+        <v>3.42043E-2</v>
+      </c>
+      <c r="D25">
+        <v>1.01362</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26">
+        <v>1425.15</v>
+      </c>
+      <c r="C26">
+        <v>2.1786900000000001E-2</v>
+      </c>
+      <c r="D26">
+        <v>1.0055099999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27">
+        <v>5423.56</v>
+      </c>
+      <c r="C27">
+        <v>6.88304E-2</v>
+      </c>
+      <c r="D27">
+        <v>1.01288</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28">
+        <v>821.12599999999998</v>
+      </c>
+      <c r="C28">
+        <v>9.6719700000000002E-3</v>
+      </c>
+      <c r="D28">
+        <v>1.1399699999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29">
+        <v>1022.44</v>
+      </c>
+      <c r="C29">
+        <v>5.7271500000000003E-3</v>
+      </c>
+      <c r="D29">
+        <v>1.4871399999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30">
+        <v>-56.566600000000001</v>
+      </c>
+      <c r="C30">
+        <v>-3.4130800000000002E-3</v>
+      </c>
+      <c r="D30">
+        <v>0.99691099999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31">
+        <v>-659.71100000000001</v>
+      </c>
+      <c r="C31">
+        <v>-1.6404100000000001E-2</v>
+      </c>
+      <c r="D31">
+        <v>0.997166</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>46</v>
+      </c>
+      <c r="E32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>47</v>
+      </c>
+      <c r="E33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35">
+        <v>266</v>
+      </c>
+      <c r="C35">
+        <v>11.184699999999999</v>
+      </c>
+      <c r="D35">
+        <v>-1.23759</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -35791,7 +37217,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -37070,7 +38496,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D279"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -41552,10 +42978,12 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <sheetData>
@@ -42325,7 +43753,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C182"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>